<commit_message>
updating BOM with aliExpress links
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sander\OneDrive\PCB\RS485-Modbus-Tiny-Sensor-Module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\michielvanwelsenaere\RS485-Modbus-Tiny-Sensor-Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{67815681-17B2-40D4-B601-26958C1C3BE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{94DB1348-60A7-40DE-BB50-36F9241FBBC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471137AC-BDB7-4E0A-A9BF-934A680EBB00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1DA501E-7FD3-4E9D-B591-418C4457BBDA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D1DA501E-7FD3-4E9D-B591-418C4457BBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Product</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -175,13 +172,37 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1068215251.html?spm=a2g0o.productlist.0.0.1e5ca144y6dBmp&amp;algo_pvid=80ccebdb-5973-4931-b90a-dfee728a65f4&amp;algo_expid=80ccebdb-5973-4931-b90a-dfee728a65f4-1&amp;btsid=0ab50f4415858253351994678edc77&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33013972369.html?spm=a2g0o.productlist.0.0.25ae390djyGrti&amp;algo_pvid=73949350-3a11-4e7e-9716-91a2fb3778bf&amp;algo_expid=73949350-3a11-4e7e-9716-91a2fb3778bf-3&amp;btsid=0ab6f81e15858255050474469e1747&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32966490820.html?spm=a2g0o.productlist.0.0.5cb5e375SYJ0QK&amp;algo_pvid=4f258cba-cd74-4f42-ad43-205c371b1b84&amp;algo_expid=4f258cba-cd74-4f42-ad43-205c371b1b84-0&amp;btsid=0ab6f83915858255934824697e4e73&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32847115923.html?spm=a2g0o.productlist.0.0.7bc147551VNoAO&amp;algo_pvid=8df103e4-73f2-4f8f-817b-f8f95c907efc&amp;algo_expid=8df103e4-73f2-4f8f-817b-f8f95c907efc-1&amp;btsid=0ab6f82415858257023173189e2d5d&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32369344670.html?spm=a2g0o.productlist.0.0.33481c2e3N4H2b&amp;algo_pvid=88cedc09-4838-4e6a-8fbb-b9fe6ef80c69&amp;algo_expid=88cedc09-4838-4e6a-8fbb-b9fe6ef80c69-4&amp;btsid=0be3764315858258286375215ec63e&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32856564094.html?spm=a2g0o.productlist.0.0.74d42da5QBNTaI&amp;algo_pvid=dc6c1b2d-0d11-482c-ab63-bf0ac9c0f492&amp;algo_expid=dc6c1b2d-0d11-482c-ab63-bf0ac9c0f492-1&amp;btsid=0ab6f81615858260205077678e29b5&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,13 +224,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,17 +254,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -247,7 +283,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -543,51 +579,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30BCD37-9A1A-40FA-9DCE-33A6F4B6022D}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="110.85546875" customWidth="1"/>
+    <col min="1" max="3" width="20.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" customWidth="1"/>
+    <col min="7" max="7" width="68.1796875" customWidth="1"/>
+    <col min="8" max="8" width="53.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>0.26100000000000001</v>
@@ -600,18 +640,21 @@
         <v>1.3050000000000002</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>0.68300000000000005</v>
@@ -623,19 +666,19 @@
         <f>D3*E3</f>
         <v>10.245000000000001</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>9.9000000000000005E-2</v>
@@ -647,19 +690,19 @@
         <f>D4*E4</f>
         <v>1.4850000000000001</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>0.82799999999999996</v>
@@ -671,19 +714,19 @@
         <f t="shared" ref="F5:F23" si="0">D5*E5</f>
         <v>24.84</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>0.315</v>
@@ -696,18 +739,21 @@
         <v>1.575</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>0.36</v>
@@ -720,18 +766,21 @@
         <v>5.3999999999999995</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>0.27900000000000003</v>
@@ -744,18 +793,21 @@
         <v>1.395</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>0.09</v>
@@ -768,18 +820,21 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>0.09</v>
@@ -792,18 +847,21 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>0.09</v>
@@ -816,18 +874,21 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>0.378</v>
@@ -840,15 +901,18 @@
         <v>1.8900000000000001</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>1206</v>
@@ -864,18 +928,18 @@
         <v>1.53</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>0.26100000000000001</v>
@@ -888,68 +952,71 @@
         <v>0.78300000000000003</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24">
         <f>SUM(F2:F23)</f>
@@ -961,6 +1028,9 @@
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{304CF3C3-773B-4DAF-AD71-6495E6850FF1}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{AAD8624F-5812-4BA1-AACA-12247F6F127E}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{AC223504-E090-4407-BA2E-9C24D20D3DA4}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{1E85891F-1DF7-444E-8686-88413F3E737B}"/>
+    <hyperlink ref="G13" r:id="rId5" xr:uid="{6A08DE33-7782-49DA-AC6F-79E223324542}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>